<commit_message>
modified:   anuncios.xlsx modified:   app.py new file:   configs/configuracoes.json renamed:    utils/mapeamento_palavras_substituir.py -> configs/mapeamentos_substituicoes_ate_60.json new file:   configs/padroes_substituicoes_nome_anuncio.json deleted:    configs/settings.json deleted:    configs/token.txt new file:   globals.py modified:   models_api/api_max.py modified:   models_api/gerar_token.py renamed:    models_api/mapeamentos.py -> models_api/mapeamentos_retorno_api.py modified:   models_excel/core.py deleted:    models_excel/padroes_substituir_nomes_anuncios.py new file:   teste.py modified:   utils/utils.py new file:   utils/utils_acertar_nome.py modified:   view/interface.py
</commit_message>
<xml_diff>
--- a/anuncios.xlsx
+++ b/anuncios.xlsx
@@ -523,7 +523,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cilindro De Roda Compatível F-1000 3.9 8V 1979-1992 Dir</t>
+          <t>Cilindro De Roda Compatível Ford F-1000 3.9 8V 1979-1992 Dr</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -594,12 +594,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Amortecedor P/ Suspensão Compatível Fiat Pulse 1.0 12V/1.3 16V/1.3 8V 2021-2025 Dianteiro Esquerdo Nakata Hg 41484</t>
+          <t>Amortecedor De Suspensão Compatível Fiat Pulse 1.0 12V/1.3 16V/1.3 8V 2021-2025 Dianteiro Esquerdo Nakata Hg 41484</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Amortecedor P/ Suspensão Compatível Pulse 1.3 16V/ 2021-2025 Diant Esq</t>
+          <t>Amortecedor Suspensão Compatível Pulse 1.3 16V/ 2021-2025 Diant Esq</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>